<commit_message>
Sync weights to Azure
</commit_message>
<xml_diff>
--- a/results/predictions/Me at the zoo.xlsx
+++ b/results/predictions/Me at the zoo.xlsx
@@ -520,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>admiration</t>
+          <t>excitement</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -547,12 +547,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>approval</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -579,12 +579,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">

</xml_diff>